<commit_message>
cleaning up old files
</commit_message>
<xml_diff>
--- a/data/archive/econ_inputs.xlsx
+++ b/data/archive/econ_inputs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/plima/dev/genomic-surveillance-voi/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/plima/dev/genomic-surveillance-voi/data/archive/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21A126F7-A952-BB46-ACF9-8D3F95F0D3B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18CAEE63-A281-9C4C-908F-D7561D4159F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19840" activeTab="2" xr2:uid="{84D0657C-0AE8-48A0-8A65-3279B3822131}"/>
   </bookViews>
@@ -393,9 +393,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -433,7 +433,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -539,7 +539,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -681,7 +681,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -4750,7 +4750,7 @@
       <pane xSplit="3" ySplit="14" topLeftCell="D15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A15" sqref="A15"/>
-      <selection pane="bottomRight" activeCell="C44" sqref="C44"/>
+      <selection pane="bottomRight" activeCell="BE16" sqref="BE16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8565,6 +8565,12 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010077E162EE38FDE5438E4954245E9CABB4" ma:contentTypeVersion="9" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="1a2fd953be0dad2bb6944c9f448122b0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="970bccd6-616f-44b9-b1d4-803881a69477" xmlns:ns3="592254e2-2768-4de2-b2b7-0b8336437af6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="bb2beca8fc03475addded86f3267ae81" ns2:_="" ns3:_="">
     <xsd:import namespace="970bccd6-616f-44b9-b1d4-803881a69477"/>
@@ -8755,12 +8761,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{398EE452-35C4-492F-85EC-E008372D567C}">
   <ds:schemaRefs>
@@ -8770,6 +8770,23 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F576E6C6-6A7D-495C-AD00-494A8E5A41FE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="970bccd6-616f-44b9-b1d4-803881a69477"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="592254e2-2768-4de2-b2b7-0b8336437af6"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{53BC0DFE-4389-4CCF-9C5B-23B8C0FDB8C2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -8786,21 +8803,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F576E6C6-6A7D-495C-AD00-494A8E5A41FE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="970bccd6-616f-44b9-b1d4-803881a69477"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="592254e2-2768-4de2-b2b7-0b8336437af6"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>